<commit_message>
Update finance data: Latest V3 Excel
</commit_message>
<xml_diff>
--- a/backend/knowledge_base/finance/dummy_supplier_sales_data_LATEST_V3.xlsx
+++ b/backend/knowledge_base/finance/dummy_supplier_sales_data_LATEST_V3.xlsx
@@ -1,36 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29725"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\coffe\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repo\Corporate AI\procure-ai-ui\backend\knowledge_base\finance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7B8BD41B-3918-4630-88D4-F16FBAD9760E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6BCBC7E-BDDD-433E-B2B7-351235E2C45B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{60342442-88B8-4CD9-B95F-A362FDDAC835}"/>
+    <workbookView xWindow="28690" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{60342442-88B8-4CD9-B95F-A362FDDAC835}"/>
   </bookViews>
   <sheets>
     <sheet name="dummy_supplier_sales_data_LATES" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">dummy_supplier_sales_data_LATES!$A$1:$F$81</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">dummy_supplier_sales_data_LATES!$A$1:$E$81</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="28">
   <si>
     <t>Supplier_Name</t>
   </si>
   <si>
-    <t>Supplier_Status</t>
-  </si>
-  <si>
     <t>Category</t>
   </si>
   <si>
@@ -46,9 +43,6 @@
     <t>Alpha Supplies</t>
   </si>
   <si>
-    <t>Active</t>
-  </si>
-  <si>
     <t>Facilities</t>
   </si>
   <si>
@@ -71,9 +65,6 @@
   </si>
   <si>
     <t>Bravo Distributors</t>
-  </si>
-  <si>
-    <t>Inactive</t>
   </si>
   <si>
     <t>December</t>
@@ -124,7 +115,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -606,7 +597,7 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
@@ -985,19 +976,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBB4F888-FD1B-4E18-8840-801ACD01507C}">
-  <dimension ref="A1:H85"/>
+  <dimension ref="A1:G85"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="19.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.1328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.46484375" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1013,481 +1004,415 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2">
+        <v>2026</v>
+      </c>
+      <c r="E2" s="2">
+        <v>37098</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3">
+        <v>2026</v>
+      </c>
+      <c r="E3" s="2">
+        <v>16395</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4">
+        <v>2026</v>
+      </c>
+      <c r="E4" s="2">
+        <v>17280</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5">
+        <v>2026</v>
+      </c>
+      <c r="E5" s="2">
+        <v>59987</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6">
+        <v>2026</v>
+      </c>
+      <c r="E6" s="2">
+        <v>25926</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7">
+        <v>2026</v>
+      </c>
+      <c r="E7" s="2">
+        <v>25379</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8">
+        <v>2026</v>
+      </c>
+      <c r="E8" s="2">
+        <v>52052</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9">
+        <v>2026</v>
+      </c>
+      <c r="E9" s="2">
+        <v>75284</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10">
+        <v>2026</v>
+      </c>
+      <c r="E10" s="2">
+        <v>52052</v>
+      </c>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11">
+        <v>2026</v>
+      </c>
+      <c r="E11" s="2">
+        <v>11006</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E2">
-        <v>2026</v>
-      </c>
-      <c r="F2" s="2">
-        <v>37098</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="D12">
+        <v>2026</v>
+      </c>
+      <c r="E12" s="2">
+        <v>35512</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13">
+        <v>2026</v>
+      </c>
+      <c r="E13" s="2">
+        <v>53520</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14">
+        <v>2026</v>
+      </c>
+      <c r="E14" s="2">
+        <v>84840</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15">
+        <v>2026</v>
+      </c>
+      <c r="E15" s="2">
+        <v>65589</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3">
-        <v>2026</v>
-      </c>
-      <c r="F3" s="2">
-        <v>16395</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E4">
-        <v>2026</v>
-      </c>
-      <c r="F4" s="2">
-        <v>17280</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5">
-        <v>2026</v>
-      </c>
-      <c r="F5" s="2">
-        <v>59987</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" t="s">
-        <v>23</v>
-      </c>
-      <c r="E6">
-        <v>2026</v>
-      </c>
-      <c r="F6" s="2">
-        <v>25926</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" t="s">
-        <v>20</v>
-      </c>
-      <c r="E7">
-        <v>2026</v>
-      </c>
-      <c r="F7" s="2">
-        <v>25379</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E8">
-        <v>2026</v>
-      </c>
-      <c r="F8" s="2">
-        <v>52052</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" t="s">
-        <v>27</v>
-      </c>
-      <c r="E9">
-        <v>2026</v>
-      </c>
-      <c r="F9" s="2">
-        <v>75284</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="C16" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16">
+        <v>2026</v>
+      </c>
+      <c r="E16" s="2">
+        <v>12331</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A17" t="s">
         <v>21</v>
-      </c>
-      <c r="B10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" t="s">
-        <v>14</v>
-      </c>
-      <c r="E10">
-        <v>2026</v>
-      </c>
-      <c r="F10" s="2">
-        <v>52052</v>
-      </c>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11" t="s">
-        <v>13</v>
-      </c>
-      <c r="E11">
-        <v>2026</v>
-      </c>
-      <c r="F11" s="2">
-        <v>11006</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" t="s">
-        <v>12</v>
-      </c>
-      <c r="D12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E12">
-        <v>2026</v>
-      </c>
-      <c r="F12" s="2">
-        <v>35512</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" t="s">
-        <v>16</v>
-      </c>
-      <c r="C13" t="s">
-        <v>22</v>
-      </c>
-      <c r="D13" t="s">
-        <v>17</v>
-      </c>
-      <c r="E13">
-        <v>2026</v>
-      </c>
-      <c r="F13" s="2">
-        <v>53520</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>24</v>
-      </c>
-      <c r="B14" t="s">
-        <v>16</v>
-      </c>
-      <c r="C14" t="s">
-        <v>12</v>
-      </c>
-      <c r="D14" t="s">
-        <v>20</v>
-      </c>
-      <c r="E14">
-        <v>2026</v>
-      </c>
-      <c r="F14" s="2">
-        <v>84840</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>24</v>
-      </c>
-      <c r="B15" t="s">
-        <v>7</v>
-      </c>
-      <c r="C15" t="s">
-        <v>22</v>
-      </c>
-      <c r="D15" t="s">
-        <v>9</v>
-      </c>
-      <c r="E15">
-        <v>2026</v>
-      </c>
-      <c r="F15" s="2">
-        <v>65589</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>24</v>
-      </c>
-      <c r="B16" t="s">
-        <v>7</v>
-      </c>
-      <c r="C16" t="s">
-        <v>8</v>
-      </c>
-      <c r="D16" t="s">
-        <v>25</v>
-      </c>
-      <c r="E16">
-        <v>2026</v>
-      </c>
-      <c r="F16" s="2">
-        <v>12331</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>24</v>
       </c>
       <c r="B17" t="s">
         <v>16</v>
       </c>
       <c r="C17" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17">
+        <v>2026</v>
+      </c>
+      <c r="E17" s="2">
+        <v>40093</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A18" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" t="s">
         <v>19</v>
       </c>
-      <c r="D17" t="s">
+      <c r="C18" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18">
+        <v>2026</v>
+      </c>
+      <c r="E18" s="2">
+        <v>90909</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A19" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" t="s">
+        <v>24</v>
+      </c>
+      <c r="D19">
+        <v>2026</v>
+      </c>
+      <c r="E19" s="2">
+        <v>39718</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A20" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" t="s">
+        <v>25</v>
+      </c>
+      <c r="D20">
+        <v>2026</v>
+      </c>
+      <c r="E20" s="2">
+        <v>61155</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" t="s">
         <v>11</v>
       </c>
-      <c r="E17">
-        <v>2026</v>
-      </c>
-      <c r="F17" s="2">
-        <v>40093</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+      <c r="D21">
+        <v>2026</v>
+      </c>
+      <c r="E21" s="2">
+        <v>23131</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A22" t="s">
         <v>26</v>
       </c>
-      <c r="B18" t="s">
-        <v>16</v>
-      </c>
-      <c r="C18" t="s">
-        <v>22</v>
-      </c>
-      <c r="D18" t="s">
-        <v>18</v>
-      </c>
-      <c r="E18">
-        <v>2026</v>
-      </c>
-      <c r="F18" s="2">
-        <v>90909</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>26</v>
-      </c>
-      <c r="B19" t="s">
-        <v>16</v>
-      </c>
-      <c r="C19" t="s">
-        <v>22</v>
-      </c>
-      <c r="D19" t="s">
-        <v>27</v>
-      </c>
-      <c r="E19">
-        <v>2026</v>
-      </c>
-      <c r="F19" s="2">
-        <v>39718</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>26</v>
-      </c>
-      <c r="B20" t="s">
-        <v>16</v>
-      </c>
-      <c r="C20" t="s">
+      <c r="B22" t="s">
         <v>10</v>
-      </c>
-      <c r="D20" t="s">
-        <v>28</v>
-      </c>
-      <c r="E20">
-        <v>2026</v>
-      </c>
-      <c r="F20" s="2">
-        <v>61155</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>26</v>
-      </c>
-      <c r="B21" t="s">
-        <v>16</v>
-      </c>
-      <c r="C21" t="s">
-        <v>22</v>
-      </c>
-      <c r="D21" t="s">
-        <v>13</v>
-      </c>
-      <c r="E21">
-        <v>2026</v>
-      </c>
-      <c r="F21" s="2">
-        <v>23131</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>29</v>
-      </c>
-      <c r="B22" t="s">
-        <v>7</v>
       </c>
       <c r="C22" t="s">
         <v>12</v>
       </c>
-      <c r="D22" t="s">
-        <v>14</v>
-      </c>
-      <c r="E22">
-        <v>2026</v>
-      </c>
-      <c r="F22" s="2">
+      <c r="D22">
+        <v>2026</v>
+      </c>
+      <c r="E22" s="2">
         <v>19371</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F27" s="3"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F31" s="3"/>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="E27" s="3"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="E31" s="3"/>
+      <c r="F31" s="1"/>
       <c r="G31" s="1"/>
-      <c r="H31" s="1"/>
-    </row>
-    <row r="33" spans="6:8" ht="16.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F33" s="3"/>
-    </row>
-    <row r="37" spans="6:8" x14ac:dyDescent="0.3">
-      <c r="F37" s="3"/>
+    </row>
+    <row r="33" spans="5:7" ht="16.8" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="E33" s="3"/>
+    </row>
+    <row r="37" spans="5:7" x14ac:dyDescent="0.45">
+      <c r="E37" s="3"/>
+      <c r="F37" s="1"/>
       <c r="G37" s="1"/>
-      <c r="H37" s="1"/>
-    </row>
-    <row r="60" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F60" s="3"/>
-    </row>
-    <row r="69" spans="6:8" x14ac:dyDescent="0.3">
-      <c r="F69" s="3"/>
-    </row>
-    <row r="76" spans="6:8" x14ac:dyDescent="0.3">
-      <c r="F76" s="3"/>
-    </row>
-    <row r="80" spans="6:8" x14ac:dyDescent="0.3">
-      <c r="F80" s="3"/>
+    </row>
+    <row r="60" spans="5:5" x14ac:dyDescent="0.45">
+      <c r="E60" s="3"/>
+    </row>
+    <row r="69" spans="5:7" x14ac:dyDescent="0.45">
+      <c r="E69" s="3"/>
+    </row>
+    <row r="76" spans="5:7" x14ac:dyDescent="0.45">
+      <c r="E76" s="3"/>
+    </row>
+    <row r="80" spans="5:7" x14ac:dyDescent="0.45">
+      <c r="E80" s="3"/>
+      <c r="F80" s="1"/>
       <c r="G80" s="1"/>
-      <c r="H80" s="1"/>
-    </row>
-    <row r="82" spans="6:8" x14ac:dyDescent="0.3">
-      <c r="F82" s="3"/>
+    </row>
+    <row r="82" spans="5:7" x14ac:dyDescent="0.45">
+      <c r="E82" s="3"/>
+      <c r="F82" s="1"/>
       <c r="G82" s="1"/>
-      <c r="H82" s="1"/>
-    </row>
-    <row r="83" spans="6:8" x14ac:dyDescent="0.3">
-      <c r="F83" s="3"/>
+    </row>
+    <row r="83" spans="5:7" x14ac:dyDescent="0.45">
+      <c r="E83" s="3"/>
+      <c r="F83" s="1"/>
       <c r="G83" s="1"/>
-      <c r="H83" s="1"/>
-    </row>
-    <row r="84" spans="6:8" x14ac:dyDescent="0.3">
-      <c r="F84" s="3"/>
+    </row>
+    <row r="84" spans="5:7" x14ac:dyDescent="0.45">
+      <c r="E84" s="3"/>
+      <c r="F84" s="1"/>
       <c r="G84" s="1"/>
-      <c r="H84" s="1"/>
-    </row>
-    <row r="85" spans="6:8" x14ac:dyDescent="0.3">
-      <c r="F85" s="3"/>
+    </row>
+    <row r="85" spans="5:7" x14ac:dyDescent="0.45">
+      <c r="E85" s="3"/>
+      <c r="F85" s="1"/>
       <c r="G85" s="1"/>
-      <c r="H85" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>